<commit_message>
1. ordered section navigator 2. added qiestion form header, hide repeated questions 3. added null labels for input controls to be compliance to HTML validation 4. added score row placeholder for dynamic calculation 5. added cookie consent 6. added StageGroupTitle in tblQuestionStage model 7. consolidate GetStage() and GetAll() to use tblQuestionStage to filter question listing
</commit_message>
<xml_diff>
--- a/VSSC Feedback June 2021 (version 1).xlsx
+++ b/VSSC Feedback June 2021 (version 1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VHAPORSUNC\source\repos\VSSC\IPRehab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA4A0BC-B318-40BE-BDE2-B3A86F693D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87C3519-04D2-4598-ACA3-26F55C2BBD74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9463" firstSheet="1" activeTab="5" xr2:uid="{D57B31B5-7152-463E-ABC6-71BF39CFCF39}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="2" activeTab="6" xr2:uid="{D57B31B5-7152-463E-ABC6-71BF39CFCF39}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Questions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="Sample - Follow Up" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
   <si>
     <t>Q 17 "Pre-hospital Living with"</t>
   </si>
@@ -203,6 +202,12 @@
   </si>
   <si>
     <t>not the same as IRF-PAI V4</t>
+  </si>
+  <si>
+    <t>GG0170Q3</t>
+  </si>
+  <si>
+    <t>GG0170Q2</t>
   </si>
 </sst>
 </file>
@@ -348,13 +353,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,7 +718,7 @@
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -728,7 +733,7 @@
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -743,7 +748,7 @@
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -758,7 +763,7 @@
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -773,7 +778,7 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -871,7 +876,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -880,19 +885,19 @@
       <c r="C1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -914,7 +919,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A2:XFD3"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,7 +943,7 @@
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -968,7 +973,7 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1034,8 +1039,8 @@
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>51</v>
+      <c r="C16" s="21" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1107,9 +1112,9 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A24" sqref="A24:XFD26"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1146,8 +1151,8 @@
       <c r="B4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>52</v>
+      <c r="C4" s="21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1161,7 +1166,7 @@
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1176,7 +1181,7 @@
       <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1191,7 +1196,7 @@
       <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1206,7 +1211,7 @@
       <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1257,7 +1262,7 @@
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1271,6 +1276,9 @@
       </c>
       <c r="B22" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1310,7 +1318,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24:XFD26"/>
     </sheetView>
   </sheetViews>
@@ -1344,10 +1352,10 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C18" sqref="C18"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1372,7 +1380,7 @@
       <c r="B2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1387,8 +1395,8 @@
       <c r="B4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>52</v>
+      <c r="C4" s="21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1402,7 +1410,7 @@
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1417,6 +1425,9 @@
       <c r="B8" s="9" t="s">
         <v>46</v>
       </c>
+      <c r="C8" s="21" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
@@ -1429,7 +1440,7 @@
       <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>